<commit_message>
Include missing data for Batten pair
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/ControledEnvironment/LincolnCE_Obs.xlsx
+++ b/Tests/Validation/Wheat/ControledEnvironment/LincolnCE_Obs.xlsx
@@ -606,6 +606,9 @@
       <c r="B11" s="2">
         <v>36639</v>
       </c>
+      <c r="E11">
+        <v>2.428060400516796</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
@@ -614,6 +617,9 @@
       <c r="B12" s="2">
         <v>36646</v>
       </c>
+      <c r="E12">
+        <v>3.601082715295001</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
@@ -622,6 +628,9 @@
       <c r="B13" s="2">
         <v>36653</v>
       </c>
+      <c r="E13">
+        <v>4.914803668672972</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
@@ -630,6 +639,9 @@
       <c r="B14" s="2">
         <v>36661</v>
       </c>
+      <c r="E14">
+        <v>5.974550507929128</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -638,6 +650,9 @@
       <c r="B15" s="2">
         <v>36667</v>
       </c>
+      <c r="E15">
+        <v>6.70534360788277</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
@@ -646,6 +661,9 @@
       <c r="B16" s="2">
         <v>36674</v>
       </c>
+      <c r="E16">
+        <v>7.385609112332162</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
@@ -654,6 +672,9 @@
       <c r="B17" s="2">
         <v>36681</v>
       </c>
+      <c r="E17">
+        <v>8.370199273368181</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
@@ -684,6 +705,9 @@
       <c r="B20" s="2">
         <v>36639</v>
       </c>
+      <c r="E20">
+        <v>2.285</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
@@ -692,6 +716,9 @@
       <c r="B21" s="2">
         <v>36646</v>
       </c>
+      <c r="E21">
+        <v>3.579664570230608</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
@@ -700,6 +727,9 @@
       <c r="B22" s="2">
         <v>36653</v>
       </c>
+      <c r="E22">
+        <v>4.735967184801382</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
@@ -708,6 +738,9 @@
       <c r="B23" s="2">
         <v>36661</v>
       </c>
+      <c r="E23">
+        <v>5.929332386363637</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
@@ -716,6 +749,9 @@
       <c r="B24" s="2">
         <v>36667</v>
       </c>
+      <c r="E24">
+        <v>6.604126984126984</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
@@ -724,6 +760,9 @@
       <c r="B25" s="2">
         <v>36674</v>
       </c>
+      <c r="E25">
+        <v>7.709947089947089</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
@@ -732,6 +771,9 @@
       <c r="B26" s="2">
         <v>36681</v>
       </c>
+      <c r="E26">
+        <v>8.594074074074072</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
@@ -752,7 +794,7 @@
         <v>36639</v>
       </c>
       <c r="E28">
-        <v>3.120248166580074</v>
+        <v>2.733696949168199</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -763,7 +805,7 @@
         <v>36646</v>
       </c>
       <c r="E29">
-        <v>4.280431539301513</v>
+        <v>4.246589485395448</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -774,7 +816,7 @@
         <v>36653</v>
       </c>
       <c r="E30">
-        <v>5.35892959870313</v>
+        <v>5.305275414013267</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -785,7 +827,7 @@
         <v>36661</v>
       </c>
       <c r="E31">
-        <v>5.970673860292429</v>
+        <v>5.923018800622259</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -796,7 +838,7 @@
         <v>36667</v>
       </c>
       <c r="E32">
-        <v>7.333638743631557</v>
+        <v>7.393218944221821</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -807,7 +849,7 @@
         <v>36674</v>
       </c>
       <c r="E33">
-        <v>7.938889123888614</v>
+        <v>7.756830019760492</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -818,7 +860,7 @@
         <v>36681</v>
       </c>
       <c r="E34">
-        <v>8.925237610053305</v>
+        <v>6.310178861788617</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -829,7 +871,7 @@
         <v>36688</v>
       </c>
       <c r="E35">
-        <v>9.470722853535353</v>
+        <v>6.685714285714285</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -906,7 +948,7 @@
         <v>36639</v>
       </c>
       <c r="E42">
-        <v>2.18912447257384</v>
+        <v>2.121700051647661</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -917,7 +959,7 @@
         <v>36646</v>
       </c>
       <c r="E43">
-        <v>3.429245283018868</v>
+        <v>3.386942675159236</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -928,7 +970,7 @@
         <v>36653</v>
       </c>
       <c r="E44">
-        <v>4.936791612694301</v>
+        <v>4.800179823737866</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -939,7 +981,7 @@
         <v>36661</v>
       </c>
       <c r="E45">
-        <v>6.249056186868686</v>
+        <v>6.027890833527469</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -950,7 +992,7 @@
         <v>36667</v>
       </c>
       <c r="E46">
-        <v>7.176190476190476</v>
+        <v>6.956493278341615</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -961,7 +1003,7 @@
         <v>36674</v>
       </c>
       <c r="E47">
-        <v>8.423809523809524</v>
+        <v>8.228275366779521</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -994,7 +1036,7 @@
         <v>36639</v>
       </c>
       <c r="E50">
-        <v>2.052940447297685</v>
+        <v>2.02566124813457</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1005,7 +1047,7 @@
         <v>36646</v>
       </c>
       <c r="E51">
-        <v>3.501275510204081</v>
+        <v>3.412988650693568</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1016,7 +1058,7 @@
         <v>36653</v>
       </c>
       <c r="E52">
-        <v>4.59433962264151</v>
+        <v>4.53639846743295</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1027,7 +1069,7 @@
         <v>36661</v>
       </c>
       <c r="E53">
-        <v>5.534394589244473</v>
+        <v>5.458722741433021</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1038,7 +1080,7 @@
         <v>36667</v>
       </c>
       <c r="E54">
-        <v>6.739725753999156</v>
+        <v>6.685076879747225</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1049,7 +1091,7 @@
         <v>36674</v>
       </c>
       <c r="E55">
-        <v>6.990567609181475</v>
+        <v>6.922885550245411</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1060,7 +1102,7 @@
         <v>36681</v>
       </c>
       <c r="E56">
-        <v>7.734101020675215</v>
+        <v>7.597444089456869</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1246,6 +1288,9 @@
       <c r="B73" s="2">
         <v>36546</v>
       </c>
+      <c r="E73">
+        <v>2.949916874480466</v>
+      </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
@@ -1254,6 +1299,9 @@
       <c r="B74" s="2">
         <v>36553</v>
       </c>
+      <c r="E74">
+        <v>3.827930824100736</v>
+      </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
@@ -1262,6 +1310,9 @@
       <c r="B75" s="2">
         <v>36558</v>
       </c>
+      <c r="E75">
+        <v>4.464450043933507</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
@@ -1270,6 +1321,9 @@
       <c r="B76" s="2">
         <v>36567</v>
       </c>
+      <c r="E76">
+        <v>5.203025010647008</v>
+      </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
@@ -1278,6 +1332,9 @@
       <c r="B77" s="2">
         <v>36574</v>
       </c>
+      <c r="E77">
+        <v>6.327372844651831</v>
+      </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
@@ -1286,6 +1343,9 @@
       <c r="B78" s="2">
         <v>36581</v>
       </c>
+      <c r="E78">
+        <v>6.978159283685803</v>
+      </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
@@ -1294,6 +1354,9 @@
       <c r="B79" s="2">
         <v>36588</v>
       </c>
+      <c r="E79">
+        <v>7.691452763876655</v>
+      </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
@@ -1302,6 +1365,9 @@
       <c r="B80" s="2">
         <v>36595</v>
       </c>
+      <c r="E80">
+        <v>8.496567390283554</v>
+      </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
@@ -1310,6 +1376,9 @@
       <c r="B81" s="2">
         <v>36602</v>
       </c>
+      <c r="E81">
+        <v>9.061967714048496</v>
+      </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
@@ -1318,6 +1387,9 @@
       <c r="B82" s="2">
         <v>36610</v>
       </c>
+      <c r="E82">
+        <v>10.17996756690134</v>
+      </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
@@ -1326,6 +1398,9 @@
       <c r="B83" s="2">
         <v>36616</v>
       </c>
+      <c r="E83">
+        <v>10.63377115675189</v>
+      </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
@@ -1335,7 +1410,7 @@
         <v>36630</v>
       </c>
       <c r="E84">
-        <v>12</v>
+        <v>11.8807570434624</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1367,6 +1442,9 @@
       <c r="B87" s="2">
         <v>36546</v>
       </c>
+      <c r="E87">
+        <v>2.894669277264863</v>
+      </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
@@ -1375,6 +1453,9 @@
       <c r="B88" s="2">
         <v>36553</v>
       </c>
+      <c r="E88">
+        <v>3.858043686174819</v>
+      </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
@@ -1383,6 +1464,9 @@
       <c r="B89" s="2">
         <v>36558</v>
       </c>
+      <c r="E89">
+        <v>4.307022483286293</v>
+      </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
@@ -1391,6 +1475,9 @@
       <c r="B90" s="2">
         <v>36567</v>
       </c>
+      <c r="E90">
+        <v>5.44758930969648</v>
+      </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
@@ -1399,6 +1486,9 @@
       <c r="B91" s="2">
         <v>36574</v>
       </c>
+      <c r="E91">
+        <v>6.505628853397302</v>
+      </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
@@ -1407,6 +1497,9 @@
       <c r="B92" s="2">
         <v>36581</v>
       </c>
+      <c r="E92">
+        <v>7.539993944227816</v>
+      </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
@@ -1415,6 +1508,9 @@
       <c r="B93" s="2">
         <v>36588</v>
       </c>
+      <c r="E93">
+        <v>8.239207487680615</v>
+      </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
@@ -1423,6 +1519,9 @@
       <c r="B94" s="2">
         <v>36595</v>
       </c>
+      <c r="E94">
+        <v>9.355048859934852</v>
+      </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
@@ -1431,6 +1530,9 @@
       <c r="B95" s="2">
         <v>36602</v>
       </c>
+      <c r="E95">
+        <v>9.542792712173821</v>
+      </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
@@ -1439,6 +1541,9 @@
       <c r="B96" s="2">
         <v>36610</v>
       </c>
+      <c r="E96">
+        <v>11.23461538461538</v>
+      </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
@@ -1447,6 +1552,9 @@
       <c r="B97" s="2">
         <v>36616</v>
       </c>
+      <c r="E97">
+        <v>11.02202455524931</v>
+      </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
@@ -1455,6 +1563,9 @@
       <c r="B98" s="2">
         <v>36630</v>
       </c>
+      <c r="E98">
+        <v>12.353125</v>
+      </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
@@ -1486,7 +1597,7 @@
         <v>36546</v>
       </c>
       <c r="E101">
-        <v>3.064375519026693</v>
+        <v>3.077334005038731</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1497,7 +1608,7 @@
         <v>36553</v>
       </c>
       <c r="E102">
-        <v>4.126303013883644</v>
+        <v>4.171586641087303</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1508,7 +1619,7 @@
         <v>36558</v>
       </c>
       <c r="E103">
-        <v>4.859282316201672</v>
+        <v>4.941293109633294</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1519,7 +1630,7 @@
         <v>36567</v>
       </c>
       <c r="E104">
-        <v>5.636901512027431</v>
+        <v>5.662674900346253</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -1530,7 +1641,7 @@
         <v>36574</v>
       </c>
       <c r="E105">
-        <v>6.894152987959807</v>
+        <v>6.955371699194276</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -1541,7 +1652,7 @@
         <v>36581</v>
       </c>
       <c r="E106">
-        <v>7.539066891512086</v>
+        <v>7.621315192743762</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -1552,7 +1663,7 @@
         <v>36588</v>
       </c>
       <c r="E107">
-        <v>8.636567773124037</v>
+        <v>8.555380972488388</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -1563,7 +1674,7 @@
         <v>36595</v>
       </c>
       <c r="E108">
-        <v>9.180154667853566</v>
+        <v>9.246606282868557</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -1574,7 +1685,7 @@
         <v>36602</v>
       </c>
       <c r="E109">
-        <v>10.75585572116479</v>
+        <v>9.569593147751606</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -1584,9 +1695,6 @@
       <c r="B110" s="2">
         <v>36610</v>
       </c>
-      <c r="E110">
-        <v>11.48925659221426</v>
-      </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
@@ -1595,9 +1703,6 @@
       <c r="B111" s="2">
         <v>36616</v>
       </c>
-      <c r="E111">
-        <v>12.21963457047641</v>
-      </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
@@ -1607,7 +1712,7 @@
         <v>36630</v>
       </c>
       <c r="E112">
-        <v>13.60035169019963</v>
+        <v>13.75519480519481</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -1618,7 +1723,7 @@
         <v>36638</v>
       </c>
       <c r="E113">
-        <v>13.41413611575108</v>
+        <v>14.05584415584416</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -1629,7 +1734,7 @@
         <v>36674</v>
       </c>
       <c r="E114">
-        <v>15.89130434782609</v>
+        <v>15.97777777777778</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -1684,7 +1789,7 @@
         <v>36546</v>
       </c>
       <c r="E119">
-        <v>3.58272414477179</v>
+        <v>3.580675740907558</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -1695,7 +1800,7 @@
         <v>36553</v>
       </c>
       <c r="E120">
-        <v>3.63905043229178</v>
+        <v>3.649148345781931</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -1706,7 +1811,7 @@
         <v>36558</v>
       </c>
       <c r="E121">
-        <v>4.874789756085082</v>
+        <v>4.834859223075668</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -1717,7 +1822,7 @@
         <v>36567</v>
       </c>
       <c r="E122">
-        <v>6.830815018315017</v>
+        <v>6.568385122964684</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -1728,7 +1833,7 @@
         <v>36574</v>
       </c>
       <c r="E123">
-        <v>8.518928004677191</v>
+        <v>8.289985371420514</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -1827,7 +1932,7 @@
         <v>36546</v>
       </c>
       <c r="E132">
-        <v>2.85531113000544</v>
+        <v>2.79945611300716</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -1838,7 +1943,7 @@
         <v>36553</v>
       </c>
       <c r="E133">
-        <v>4.008620918892745</v>
+        <v>3.881544929736314</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -1849,7 +1954,7 @@
         <v>36558</v>
       </c>
       <c r="E134">
-        <v>4.683063969502782</v>
+        <v>4.518611548492419</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -1860,7 +1965,7 @@
         <v>36567</v>
       </c>
       <c r="E135">
-        <v>5.289699321621002</v>
+        <v>5.183130897343855</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -1871,7 +1976,7 @@
         <v>36574</v>
       </c>
       <c r="E136">
-        <v>6.461893579972173</v>
+        <v>6.315291904060707</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -1882,7 +1987,7 @@
         <v>36581</v>
       </c>
       <c r="E137">
-        <v>6.940492443564277</v>
+        <v>6.78329595459256</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -1893,7 +1998,7 @@
         <v>36588</v>
       </c>
       <c r="E138">
-        <v>7.644492906854274</v>
+        <v>7.493957516018458</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -1904,7 +2009,7 @@
         <v>36595</v>
       </c>
       <c r="E139">
-        <v>8.486113788677581</v>
+        <v>8.34476246133107</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -1915,7 +2020,7 @@
         <v>36602</v>
       </c>
       <c r="E140">
-        <v>9.0155232076504</v>
+        <v>8.905697177312417</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -1926,7 +2031,7 @@
         <v>36610</v>
       </c>
       <c r="E141">
-        <v>10.37313875182323</v>
+        <v>10.34781949934124</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -1937,7 +2042,7 @@
         <v>36616</v>
       </c>
       <c r="E142">
-        <v>10.19104676783664</v>
+        <v>10.11325428194993</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2057,6 +2162,9 @@
       <c r="B153" s="2">
         <v>36641</v>
       </c>
+      <c r="E153">
+        <v>2.77875</v>
+      </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
@@ -2065,6 +2173,9 @@
       <c r="B154" s="2">
         <v>36648</v>
       </c>
+      <c r="E154">
+        <v>4.354672549019607</v>
+      </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
@@ -2073,6 +2184,9 @@
       <c r="B155" s="2">
         <v>36653</v>
       </c>
+      <c r="E155">
+        <v>4.602333333333334</v>
+      </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="1" t="s">
@@ -2092,6 +2206,9 @@
       <c r="B157" s="2">
         <v>36641</v>
       </c>
+      <c r="E157">
+        <v>3.513480918489432</v>
+      </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1" t="s">
@@ -2100,6 +2217,9 @@
       <c r="B158" s="2">
         <v>36648</v>
       </c>
+      <c r="E158">
+        <v>4.86938983845437</v>
+      </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
@@ -2108,6 +2228,9 @@
       <c r="B159" s="2">
         <v>36653</v>
       </c>
+      <c r="E159">
+        <v>5.238481221538957</v>
+      </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
@@ -2116,6 +2239,9 @@
       <c r="B160" s="2">
         <v>36659</v>
       </c>
+      <c r="E160">
+        <v>5.913443830570903</v>
+      </c>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
@@ -2147,7 +2273,7 @@
         <v>36641</v>
       </c>
       <c r="E163">
-        <v>3.323946706887883</v>
+        <v>2.909907446501934</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -2158,7 +2284,7 @@
         <v>36648</v>
       </c>
       <c r="E164">
-        <v>4.402277807138626</v>
+        <v>4.503084953055913</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -2169,7 +2295,7 @@
         <v>36653</v>
       </c>
       <c r="E165">
-        <v>5.256666195998101</v>
+        <v>5.456542407603402</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -2180,7 +2306,7 @@
         <v>36659</v>
       </c>
       <c r="E166">
-        <v>6.052695606280512</v>
+        <v>6.277260356720665</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -2191,7 +2317,7 @@
         <v>36666</v>
       </c>
       <c r="E167">
-        <v>6.565958979494665</v>
+        <v>6.802236905136427</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -2213,7 +2339,7 @@
         <v>36641</v>
       </c>
       <c r="E169">
-        <v>2.915552044666688</v>
+        <v>2.729770442922836</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -2224,7 +2350,7 @@
         <v>36648</v>
       </c>
       <c r="E170">
-        <v>4.743010508567753</v>
+        <v>4.614949236065259</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -2235,7 +2361,7 @@
         <v>36653</v>
       </c>
       <c r="E171">
-        <v>5.832747363134104</v>
+        <v>5.693032606646981</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -2257,7 +2383,7 @@
         <v>36641</v>
       </c>
       <c r="E173">
-        <v>2.815234522477118</v>
+        <v>6.939375453885258</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -2268,7 +2394,7 @@
         <v>36648</v>
       </c>
       <c r="E174">
-        <v>4.322749860746435</v>
+        <v>3.655773420479303</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -2278,9 +2404,6 @@
       <c r="B175" s="2">
         <v>36653</v>
       </c>
-      <c r="E175">
-        <v>5.056834744225061</v>
-      </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
@@ -2289,9 +2412,6 @@
       <c r="B176" s="2">
         <v>36659</v>
       </c>
-      <c r="E176">
-        <v>5.880703114774386</v>
-      </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
@@ -2301,7 +2421,7 @@
         <v>36666</v>
       </c>
       <c r="E177">
-        <v>6.746069360415887</v>
+        <v>7.078125</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -2465,6 +2585,9 @@
       <c r="B192" s="2">
         <v>36533</v>
       </c>
+      <c r="E192">
+        <v>1.005691339184544</v>
+      </c>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
@@ -2473,6 +2596,9 @@
       <c r="B193" s="2">
         <v>36540</v>
       </c>
+      <c r="E193">
+        <v>2.844458049379705</v>
+      </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1" t="s">
@@ -2481,6 +2607,9 @@
       <c r="B194" s="2">
         <v>36547</v>
       </c>
+      <c r="E194">
+        <v>3.875892214906213</v>
+      </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
@@ -2489,6 +2618,9 @@
       <c r="B195" s="2">
         <v>36554</v>
       </c>
+      <c r="E195">
+        <v>5.194303974999472</v>
+      </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1" t="s">
@@ -2497,6 +2629,9 @@
       <c r="B196" s="2">
         <v>36561</v>
       </c>
+      <c r="E196">
+        <v>6.779204073692867</v>
+      </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1" t="s">
@@ -2516,6 +2651,9 @@
       <c r="B198" s="2">
         <v>36533</v>
       </c>
+      <c r="E198">
+        <v>1.532421694914059</v>
+      </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
@@ -2524,6 +2662,9 @@
       <c r="B199" s="2">
         <v>36540</v>
       </c>
+      <c r="E199">
+        <v>2.616386858944526</v>
+      </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
@@ -2532,6 +2673,9 @@
       <c r="B200" s="2">
         <v>36547</v>
       </c>
+      <c r="E200">
+        <v>4.972746375102701</v>
+      </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
@@ -2540,6 +2684,9 @@
       <c r="B201" s="2">
         <v>36554</v>
       </c>
+      <c r="E201">
+        <v>4.899201261515694</v>
+      </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1" t="s">
@@ -2548,6 +2695,9 @@
       <c r="B202" s="2">
         <v>36561</v>
       </c>
+      <c r="E202">
+        <v>6.058783771033148</v>
+      </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
@@ -2556,6 +2706,9 @@
       <c r="B203" s="2">
         <v>36568</v>
       </c>
+      <c r="E203">
+        <v>7.106542821319646</v>
+      </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
@@ -2564,6 +2717,9 @@
       <c r="B204" s="2">
         <v>36582</v>
       </c>
+      <c r="E204">
+        <v>8.479433878814683</v>
+      </c>
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
@@ -2571,6 +2727,9 @@
       </c>
       <c r="B205" s="2">
         <v>36597</v>
+      </c>
+      <c r="E205">
+        <v>9.34078584891982</v>
       </c>
     </row>
     <row r="206" spans="1:5">

</xml_diff>